<commit_message>
conditions added to KG
</commit_message>
<xml_diff>
--- a/mappings/solarchem-mapping.xlsx
+++ b/mappings/solarchem-mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-ontology/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B843FD-AA4D-B14D-BFBE-385C96D15484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97360CB-4F2C-5C47-B863-3B8E0BEFE8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="54160" yWindow="-10300" windowWidth="25840" windowHeight="28300" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <author>tc={44F07727-749F-3C47-BA2B-19F03CB8B7C7}</author>
   </authors>
   <commentList>
-    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{44F07727-749F-3C47-BA2B-19F03CB8B7C7}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{44F07727-749F-3C47-BA2B-19F03CB8B7C7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="164">
   <si>
     <t>Prefix</t>
   </si>
@@ -406,13 +406,154 @@
   </si>
   <si>
     <t>http://w3id.org/solar/i/Input/Dye/{ID}-{Dyes}</t>
+  </si>
+  <si>
+    <t>solar:depositionMethod</t>
+  </si>
+  <si>
+    <t>{Deposition_method}</t>
+  </si>
+  <si>
+    <t>solar:hasBandGap</t>
+  </si>
+  <si>
+    <t>solar:hasSurfaceArea</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/SurfaceArea/{ID}-{Catalyst}</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/BandGap/{ID}-{Catalyst}</t>
+  </si>
+  <si>
+    <t>BANDGAP</t>
+  </si>
+  <si>
+    <t>SURFACEAREA</t>
+  </si>
+  <si>
+    <t>solar:BandGap</t>
+  </si>
+  <si>
+    <t>solar:SurfaceArea</t>
+  </si>
+  <si>
+    <t>{BET_m2_g}</t>
+  </si>
+  <si>
+    <t>{Eg_eV}</t>
+  </si>
+  <si>
+    <t>unit:EV</t>
+  </si>
+  <si>
+    <t>unit:M2-PER-GM</t>
+  </si>
+  <si>
+    <t>solar:hasCondition</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/Condition/pH/{ID}</t>
+  </si>
+  <si>
+    <t>solar:hasLightSource</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/Condition/LightSource/{ID}</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/Condition/Reactor/{ID}</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/Condition/Pressure/{ID}</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/Condition/Temperature/{ID}</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/Condition/Time/{ID}</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>REACTOR</t>
+  </si>
+  <si>
+    <t>PRESSURE</t>
+  </si>
+  <si>
+    <t>TEMPERATURE</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>solar:pHCondition</t>
+  </si>
+  <si>
+    <t>solarpc:ReactorCondition</t>
+  </si>
+  <si>
+    <t>solar:PressureCondition</t>
+  </si>
+  <si>
+    <t>solar:TemperatureCondition</t>
+  </si>
+  <si>
+    <t>solar:TimeCondition</t>
+  </si>
+  <si>
+    <t>{ph_value}</t>
+  </si>
+  <si>
+    <t>solarpc:reactorVolume</t>
+  </si>
+  <si>
+    <t>{Reactor_Volume_l}</t>
+  </si>
+  <si>
+    <t>{P_bar}</t>
+  </si>
+  <si>
+    <t>{T_C}</t>
+  </si>
+  <si>
+    <t>{Reaction_time_h}</t>
+  </si>
+  <si>
+    <t>unit:HR</t>
+  </si>
+  <si>
+    <t>unit:BAR</t>
+  </si>
+  <si>
+    <t>unit:DEG_C</t>
+  </si>
+  <si>
+    <t>unit:L</t>
+  </si>
+  <si>
+    <t>unit:PH</t>
+  </si>
+  <si>
+    <t>rdf:type</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/o/pc#{Reactor_type}Reactor</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/o/core#{Reaction_medium}Medium</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/o/core#{Operation_mode}Mode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -457,12 +598,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -490,7 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -504,8 +639,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -827,7 +960,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D19" dT="2024-03-22T16:26:13.29" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{44F07727-749F-3C47-BA2B-19F03CB8B7C7}">
+  <threadedComment ref="D12" dT="2024-03-22T16:26:13.29" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{44F07727-749F-3C47-BA2B-19F03CB8B7C7}">
     <text>Should be float, cannot bc data contains sometimes strings</text>
   </threadedComment>
 </ThreadedComments>
@@ -838,7 +971,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1006,10 +1139,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E19" sqref="E19:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1099,7 +1232,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>35</v>
@@ -1110,7 +1243,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>37</v>
@@ -1121,7 +1254,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>35</v>
@@ -1132,7 +1265,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>37</v>
@@ -1143,7 +1276,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>35</v>
@@ -1154,7 +1287,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>37</v>
@@ -1165,7 +1298,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>35</v>
@@ -1176,7 +1309,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>37</v>
@@ -1187,7 +1320,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>35</v>
@@ -1198,7 +1331,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>37</v>
@@ -1209,7 +1342,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>35</v>
@@ -1220,12 +1353,166 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1237,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C10" sqref="C9:C10"/>
+      <selection activeCell="A13" sqref="A13:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1297,83 +1584,167 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>83</v>
+      <c r="A5" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
         <v>67</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
         <v>67</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>116</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F1F592FE-66EF-D044-98C4-B07EFAF6846A}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{329341A0-A072-9242-8F6F-A7B5E8616EED}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{02AE9908-CF19-CB41-8387-762706A65FB6}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{4B69325E-4848-5C4A-97E8-083D91448168}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{6EF885FD-DCB7-D742-A7EE-E1398ABBDE76}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{E84559C3-422D-E949-A0E2-77EA15D80EEC}"/>
-    <hyperlink ref="C7" r:id="rId7" xr:uid="{A141179C-E949-524D-B44F-359B38E10D12}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{FD31A938-338A-0349-B696-E419DD58C7DB}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{8614587D-753C-C145-A81C-DA020E193AD7}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{4B69325E-4848-5C4A-97E8-083D91448168}"/>
+    <hyperlink ref="C10" r:id="rId5" xr:uid="{6EF885FD-DCB7-D742-A7EE-E1398ABBDE76}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{E84559C3-422D-E949-A0E2-77EA15D80EEC}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{A141179C-E949-524D-B44F-359B38E10D12}"/>
+    <hyperlink ref="C11" r:id="rId8" xr:uid="{FD31A938-338A-0349-B696-E419DD58C7DB}"/>
+    <hyperlink ref="C12" r:id="rId9" xr:uid="{8614587D-753C-C145-A81C-DA020E193AD7}"/>
+    <hyperlink ref="C5" r:id="rId10" xr:uid="{A9E9C9C6-B4B7-7B45-B322-7FED04CC7F6F}"/>
+    <hyperlink ref="C6" r:id="rId11" xr:uid="{0B8F8956-6FC1-7148-8FCF-BD724E0E6194}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{DB791FD6-560D-BC4B-95CF-C462CC61462D}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{9CDFBDF7-DF8A-F247-9234-17EC239F807D}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{765CBB11-AA14-E145-8CC6-3063571D0F24}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{2CA5367A-ADF2-3948-A151-F9ED43232B41}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{AF45DD89-DCAB-9D47-82E7-E1514F724422}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1382,17 +1753,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" customWidth="1"/>
-    <col min="3" max="3" width="40.5" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" customWidth="1"/>
@@ -1553,16 +1924,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>70</v>
+        <v>79</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -1570,13 +1938,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>96</v>
+        <v>68</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>70</v>
@@ -1587,30 +1955,28 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>70</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>106</v>
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>89</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>70</v>
@@ -1621,47 +1987,43 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>70</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>70</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>70</v>
@@ -1675,10 +2037,13 @@
         <v>66</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>80</v>
+        <v>120</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -1686,16 +2051,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -1703,31 +2068,33 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="7"/>
+        <v>129</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>89</v>
+        <v>73</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>127</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1735,15 +2102,17 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="7"/>
+        <v>130</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -1759,6 +2128,9 @@
         <v>91</v>
       </c>
       <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
@@ -1773,6 +2145,9 @@
       <c r="D23" s="7" t="s">
         <v>70</v>
       </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
@@ -1787,6 +2162,9 @@
       <c r="D24" s="7" t="s">
         <v>98</v>
       </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
@@ -1988,20 +2366,395 @@
         <v>98</v>
       </c>
     </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" xr:uid="{33CD0375-FDC4-864D-8BAE-CF58136577F6}"/>
-    <hyperlink ref="C11" r:id="rId2" xr:uid="{87955B5B-4B6D-4B4A-B115-3F447052E311}"/>
-    <hyperlink ref="C14" r:id="rId3" xr:uid="{3D40A9A3-79A8-4048-A619-0101D21BBBDB}"/>
-    <hyperlink ref="C12" r:id="rId4" xr:uid="{DF6AE900-F5E5-1A46-90FE-9B17C12CD5EA}"/>
-    <hyperlink ref="C13" r:id="rId5" xr:uid="{26286F07-CF01-3D4F-AF7E-24B1DFF4CAC5}"/>
-    <hyperlink ref="C15" r:id="rId6" xr:uid="{250FC759-8E91-AD4E-BB93-AAF3872DC404}"/>
-    <hyperlink ref="C16" r:id="rId7" xr:uid="{5D2E891D-0452-324E-AC63-3B5EB8FCC576}"/>
+    <hyperlink ref="C40" r:id="rId1" xr:uid="{33CD0375-FDC4-864D-8BAE-CF58136577F6}"/>
+    <hyperlink ref="C41" r:id="rId2" xr:uid="{87955B5B-4B6D-4B4A-B115-3F447052E311}"/>
+    <hyperlink ref="C44" r:id="rId3" xr:uid="{3D40A9A3-79A8-4048-A619-0101D21BBBDB}"/>
+    <hyperlink ref="C42" r:id="rId4" xr:uid="{DF6AE900-F5E5-1A46-90FE-9B17C12CD5EA}"/>
+    <hyperlink ref="C43" r:id="rId5" xr:uid="{26286F07-CF01-3D4F-AF7E-24B1DFF4CAC5}"/>
+    <hyperlink ref="C45" r:id="rId6" xr:uid="{250FC759-8E91-AD4E-BB93-AAF3872DC404}"/>
+    <hyperlink ref="C46" r:id="rId7" xr:uid="{5D2E891D-0452-324E-AC63-3B5EB8FCC576}"/>
+    <hyperlink ref="C16" r:id="rId8" xr:uid="{B83A9430-8469-3340-8A32-6DDD9D53D7BD}"/>
+    <hyperlink ref="C17" r:id="rId9" xr:uid="{699A6F69-F379-0348-B5C9-C25D7DB140FB}"/>
+    <hyperlink ref="C47" r:id="rId10" xr:uid="{EFCC2B08-8773-C547-9417-6D50A357579D}"/>
+    <hyperlink ref="C48" r:id="rId11" xr:uid="{4ED7AA7D-0161-9048-913F-4E262F489078}"/>
+    <hyperlink ref="C49" r:id="rId12" xr:uid="{055C092E-EA3C-784C-9752-B62AF65DB27F}"/>
+    <hyperlink ref="C50" r:id="rId13" xr:uid="{D4B94815-2A3D-554A-9A3A-D6C41768932F}"/>
+    <hyperlink ref="C51" r:id="rId14" xr:uid="{B9A4BC97-C4E7-CB40-BDEE-3FC54B1A15F8}"/>
+    <hyperlink ref="C52" r:id="rId15" xr:uid="{1A254817-AA29-4349-9F3D-1F08E4B7BC6D}"/>
+    <hyperlink ref="C59" r:id="rId16" location="{Reactor_type}Reactor" xr:uid="{0AB9E7B4-D674-2E47-9B72-341D1022B491}"/>
+    <hyperlink ref="C53" r:id="rId17" location="{Reaction_medium}Medium" xr:uid="{9FFFB41F-40DA-E844-8105-33FA71783875}"/>
+    <hyperlink ref="C54" r:id="rId18" location="{Operation_mode}Mode" xr:uid="{E49C1ABB-2410-D945-BAD5-E813751ECA22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId8"/>
+  <legacyDrawing r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
lightsources and outputs added, the latter separated in another mapping file
</commit_message>
<xml_diff>
--- a/mappings/solarchem-mapping.xlsx
+++ b/mappings/solarchem-mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/GitHub/solarchem-ontology/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97360CB-4F2C-5C47-B863-3B8E0BEFE8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F069437-B2D6-4E48-BBC4-181EFB03A12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="54160" yWindow="-10300" windowWidth="25840" windowHeight="28300" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,6 +40,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={44F07727-749F-3C47-BA2B-19F03CB8B7C7}</author>
+    <author>tc={16A91D93-63D0-AF4D-B9FC-79B454B39BC8}</author>
+    <author>tc={695439C3-0C5E-F940-94A3-9E975DD569EF}</author>
   </authors>
   <commentList>
     <comment ref="D12" authorId="0" shapeId="0" xr:uid="{44F07727-749F-3C47-BA2B-19F03CB8B7C7}">
@@ -50,12 +52,29 @@
     Should be float, cannot bc data contains sometimes strings</t>
       </text>
     </comment>
+    <comment ref="B42" authorId="1" shapeId="0" xr:uid="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    No está en la onto, tiene valor especial con respecto al resto de inputs
+</t>
+      </text>
+    </comment>
+    <comment ref="B73" authorId="2" shapeId="0" xr:uid="{695439C3-0C5E-F940-94A3-9E975DD569EF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    No encuentro el campo en los datos, igual se calcula on the fly?</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="193">
   <si>
     <t>Prefix</t>
   </si>
@@ -547,13 +566,100 @@
   </si>
   <si>
     <t>http://w3id.org/solar/o/core#{Operation_mode}Mode</t>
+  </si>
+  <si>
+    <t>LIGHT</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_</t>
+  </si>
+  <si>
+    <t>obi</t>
+  </si>
+  <si>
+    <t>obi:0400065</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/o/core#{Light_source}LightSource</t>
+  </si>
+  <si>
+    <t>solar:hasLamp</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/o/core#{Lamp}Lamp</t>
+  </si>
+  <si>
+    <t>solar:hasWavelength</t>
+  </si>
+  <si>
+    <t>solar:hasIrradiance</t>
+  </si>
+  <si>
+    <t>solar:hasPower</t>
+  </si>
+  <si>
+    <t>solar:hasIlluminatedArea</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/o/core#{Wavelength_nm}WL</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/IlluminatedArea/{ID}</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/Power/{ID}</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/Irradiance/{ID}</t>
+  </si>
+  <si>
+    <t>POWER</t>
+  </si>
+  <si>
+    <t>IRRADIANCE</t>
+  </si>
+  <si>
+    <t>solar:Power</t>
+  </si>
+  <si>
+    <t>solar:Irradiance</t>
+  </si>
+  <si>
+    <t>{Power_W}</t>
+  </si>
+  <si>
+    <t>{Light_Intensity_W_m2}</t>
+  </si>
+  <si>
+    <t>unit:W</t>
+  </si>
+  <si>
+    <t>unit:W-PER-M2</t>
+  </si>
+  <si>
+    <t>REDUCTANT</t>
+  </si>
+  <si>
+    <t>{Reductant}</t>
+  </si>
+  <si>
+    <t>solarpc:Reductant</t>
+  </si>
+  <si>
+    <t>solarpc:reductantRatio</t>
+  </si>
+  <si>
+    <t>{CO2_H2O_reductant_ratio}</t>
+  </si>
+  <si>
+    <t>http://w3id.org/solar/i/Input/Reductant/{ID}-{Reductant}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -595,6 +701,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -963,15 +1075,22 @@
   <threadedComment ref="D12" dT="2024-03-22T16:26:13.29" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{44F07727-749F-3C47-BA2B-19F03CB8B7C7}">
     <text>Should be float, cannot bc data contains sometimes strings</text>
   </threadedComment>
+  <threadedComment ref="B42" dT="2024-03-23T15:13:35.29" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{16A91D93-63D0-AF4D-B9FC-79B454B39BC8}">
+    <text xml:space="preserve">No está en la onto, tiene valor especial con respecto al resto de inputs
+</text>
+  </threadedComment>
+  <threadedComment ref="B73" dT="2024-03-23T15:08:06.85" personId="{38DFC2E4-73EA-D74C-967B-80CBA1CEA104}" id="{695439C3-0C5E-F940-94A3-9E975DD569EF}">
+    <text>No encuentro el campo en los datos, igual se calcula on the fly?</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1103,21 +1222,29 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B17" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="6"/>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B16" r:id="rId1" xr:uid="{F8754CBA-ECDB-4444-8F8F-EBA6BEFBBCF3}"/>
+    <hyperlink ref="B17" r:id="rId1" xr:uid="{F8754CBA-ECDB-4444-8F8F-EBA6BEFBBCF3}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{4E1D75EA-0423-7E40-BBCD-B6BD079FA83E}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{D60B0DDB-58EA-FA48-A2CD-CBE7C55549A6}"/>
     <hyperlink ref="B4" r:id="rId4" xr:uid="{E6258B07-1D09-D64E-8845-A7B81A5A2C61}"/>
@@ -1131,6 +1258,7 @@
     <hyperlink ref="B12" r:id="rId12" xr:uid="{8267D84A-C1CB-034F-A51A-3E4AF338730F}"/>
     <hyperlink ref="B13" r:id="rId13" xr:uid="{B3279D13-FFF6-2B4F-AEBD-340BDE50F7B5}"/>
     <hyperlink ref="B14" r:id="rId14" xr:uid="{756BE30A-ED1A-4B47-9579-24C4F70F99E0}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{50D40236-C10B-CC4C-BBCD-6777D6B8823C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1139,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:E23"/>
+      <selection activeCell="B24" sqref="B24:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1408,7 +1536,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>35</v>
@@ -1419,7 +1547,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>37</v>
@@ -1430,7 +1558,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>35</v>
@@ -1441,7 +1569,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>37</v>
@@ -1452,7 +1580,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>35</v>
@@ -1463,7 +1591,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>37</v>
@@ -1474,7 +1602,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>35</v>
@@ -1485,7 +1613,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>37</v>
@@ -1496,7 +1624,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>35</v>
@@ -1507,12 +1635,100 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1524,10 +1740,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A17"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1673,61 +1889,105 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>67</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>132</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>143</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>148</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C18" s="8" t="s">
         <v>138</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{F1F592FE-66EF-D044-98C4-B07EFAF6846A}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{329341A0-A072-9242-8F6F-A7B5E8616EED}"/>
@@ -1740,11 +2000,16 @@
     <hyperlink ref="C12" r:id="rId9" xr:uid="{8614587D-753C-C145-A81C-DA020E193AD7}"/>
     <hyperlink ref="C5" r:id="rId10" xr:uid="{A9E9C9C6-B4B7-7B45-B322-7FED04CC7F6F}"/>
     <hyperlink ref="C6" r:id="rId11" xr:uid="{0B8F8956-6FC1-7148-8FCF-BD724E0E6194}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{DB791FD6-560D-BC4B-95CF-C462CC61462D}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{9CDFBDF7-DF8A-F247-9234-17EC239F807D}"/>
-    <hyperlink ref="C15" r:id="rId14" xr:uid="{765CBB11-AA14-E145-8CC6-3063571D0F24}"/>
-    <hyperlink ref="C16" r:id="rId15" xr:uid="{2CA5367A-ADF2-3948-A151-F9ED43232B41}"/>
-    <hyperlink ref="C17" r:id="rId16" xr:uid="{AF45DD89-DCAB-9D47-82E7-E1514F724422}"/>
+    <hyperlink ref="C14" r:id="rId12" xr:uid="{DB791FD6-560D-BC4B-95CF-C462CC61462D}"/>
+    <hyperlink ref="C15" r:id="rId13" xr:uid="{9CDFBDF7-DF8A-F247-9234-17EC239F807D}"/>
+    <hyperlink ref="C16" r:id="rId14" xr:uid="{765CBB11-AA14-E145-8CC6-3063571D0F24}"/>
+    <hyperlink ref="C17" r:id="rId15" xr:uid="{2CA5367A-ADF2-3948-A151-F9ED43232B41}"/>
+    <hyperlink ref="C18" r:id="rId16" xr:uid="{AF45DD89-DCAB-9D47-82E7-E1514F724422}"/>
+    <hyperlink ref="C19" r:id="rId17" xr:uid="{C6281ADE-B007-FF43-987D-BC199502F4A9}"/>
+    <hyperlink ref="C20:C21" r:id="rId18" display="http://w3id.org/solar/i/IlluminatedArea/{ID}" xr:uid="{383A6330-6BEE-9442-B294-451EF5F17054}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{809DAE46-CFDD-1347-93E9-73C62A907742}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{A8085152-3BE9-844F-BD28-D23B3F3D0675}"/>
+    <hyperlink ref="C13" r:id="rId21" xr:uid="{CA6E68C4-20B1-9248-AA29-D1A87184FF3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1753,10 +2018,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2368,27 +2633,25 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>40</v>
+        <v>187</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>70</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>40</v>
+        <v>187</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>96</v>
+        <v>68</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>189</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>70</v>
@@ -2396,16 +2659,16 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>40</v>
+        <v>187</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>105</v>
+        <v>190</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -2416,7 +2679,7 @@
         <v>64</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>70</v>
@@ -2430,7 +2693,7 @@
         <v>64</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>70</v>
@@ -2444,7 +2707,7 @@
         <v>64</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>70</v>
@@ -2458,7 +2721,7 @@
         <v>64</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>70</v>
@@ -2469,10 +2732,10 @@
         <v>40</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>133</v>
+        <v>64</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>134</v>
+        <v>97</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>70</v>
@@ -2483,10 +2746,10 @@
         <v>40</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>131</v>
+        <v>64</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>70</v>
@@ -2497,10 +2760,10 @@
         <v>40</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>131</v>
+        <v>64</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>70</v>
@@ -2511,10 +2774,10 @@
         <v>40</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>131</v>
+        <v>64</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>136</v>
+        <v>192</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>70</v>
@@ -2525,10 +2788,10 @@
         <v>40</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>70</v>
@@ -2542,7 +2805,7 @@
         <v>131</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>70</v>
@@ -2556,7 +2819,7 @@
         <v>131</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>70</v>
@@ -2570,7 +2833,7 @@
         <v>131</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>70</v>
@@ -2578,27 +2841,27 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>149</v>
+        <v>131</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>159</v>
+        <v>131</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>138</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>70</v>
@@ -2606,27 +2869,27 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>151</v>
+        <v>131</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>162</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>158</v>
+        <v>131</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>163</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>70</v>
@@ -2634,69 +2897,69 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>161</v>
+        <v>73</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>149</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>157</v>
+        <v>160</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>161</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>70</v>
@@ -2704,13 +2967,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>98</v>
@@ -2718,43 +2981,247 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C65" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D69" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D79" s="7" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C40" r:id="rId1" xr:uid="{33CD0375-FDC4-864D-8BAE-CF58136577F6}"/>
-    <hyperlink ref="C41" r:id="rId2" xr:uid="{87955B5B-4B6D-4B4A-B115-3F447052E311}"/>
-    <hyperlink ref="C44" r:id="rId3" xr:uid="{3D40A9A3-79A8-4048-A619-0101D21BBBDB}"/>
-    <hyperlink ref="C42" r:id="rId4" xr:uid="{DF6AE900-F5E5-1A46-90FE-9B17C12CD5EA}"/>
-    <hyperlink ref="C43" r:id="rId5" xr:uid="{26286F07-CF01-3D4F-AF7E-24B1DFF4CAC5}"/>
-    <hyperlink ref="C45" r:id="rId6" xr:uid="{250FC759-8E91-AD4E-BB93-AAF3872DC404}"/>
-    <hyperlink ref="C46" r:id="rId7" xr:uid="{5D2E891D-0452-324E-AC63-3B5EB8FCC576}"/>
+    <hyperlink ref="C43" r:id="rId1" xr:uid="{33CD0375-FDC4-864D-8BAE-CF58136577F6}"/>
+    <hyperlink ref="C44" r:id="rId2" xr:uid="{87955B5B-4B6D-4B4A-B115-3F447052E311}"/>
+    <hyperlink ref="C47" r:id="rId3" xr:uid="{3D40A9A3-79A8-4048-A619-0101D21BBBDB}"/>
+    <hyperlink ref="C45" r:id="rId4" xr:uid="{DF6AE900-F5E5-1A46-90FE-9B17C12CD5EA}"/>
+    <hyperlink ref="C46" r:id="rId5" xr:uid="{26286F07-CF01-3D4F-AF7E-24B1DFF4CAC5}"/>
+    <hyperlink ref="C48" r:id="rId6" xr:uid="{250FC759-8E91-AD4E-BB93-AAF3872DC404}"/>
+    <hyperlink ref="C50" r:id="rId7" xr:uid="{5D2E891D-0452-324E-AC63-3B5EB8FCC576}"/>
     <hyperlink ref="C16" r:id="rId8" xr:uid="{B83A9430-8469-3340-8A32-6DDD9D53D7BD}"/>
     <hyperlink ref="C17" r:id="rId9" xr:uid="{699A6F69-F379-0348-B5C9-C25D7DB140FB}"/>
-    <hyperlink ref="C47" r:id="rId10" xr:uid="{EFCC2B08-8773-C547-9417-6D50A357579D}"/>
-    <hyperlink ref="C48" r:id="rId11" xr:uid="{4ED7AA7D-0161-9048-913F-4E262F489078}"/>
-    <hyperlink ref="C49" r:id="rId12" xr:uid="{055C092E-EA3C-784C-9752-B62AF65DB27F}"/>
-    <hyperlink ref="C50" r:id="rId13" xr:uid="{D4B94815-2A3D-554A-9A3A-D6C41768932F}"/>
-    <hyperlink ref="C51" r:id="rId14" xr:uid="{B9A4BC97-C4E7-CB40-BDEE-3FC54B1A15F8}"/>
-    <hyperlink ref="C52" r:id="rId15" xr:uid="{1A254817-AA29-4349-9F3D-1F08E4B7BC6D}"/>
-    <hyperlink ref="C59" r:id="rId16" location="{Reactor_type}Reactor" xr:uid="{0AB9E7B4-D674-2E47-9B72-341D1022B491}"/>
-    <hyperlink ref="C53" r:id="rId17" location="{Reaction_medium}Medium" xr:uid="{9FFFB41F-40DA-E844-8105-33FA71783875}"/>
-    <hyperlink ref="C54" r:id="rId18" location="{Operation_mode}Mode" xr:uid="{E49C1ABB-2410-D945-BAD5-E813751ECA22}"/>
+    <hyperlink ref="C51" r:id="rId10" xr:uid="{EFCC2B08-8773-C547-9417-6D50A357579D}"/>
+    <hyperlink ref="C52" r:id="rId11" xr:uid="{4ED7AA7D-0161-9048-913F-4E262F489078}"/>
+    <hyperlink ref="C53" r:id="rId12" xr:uid="{055C092E-EA3C-784C-9752-B62AF65DB27F}"/>
+    <hyperlink ref="C54" r:id="rId13" xr:uid="{D4B94815-2A3D-554A-9A3A-D6C41768932F}"/>
+    <hyperlink ref="C55" r:id="rId14" xr:uid="{B9A4BC97-C4E7-CB40-BDEE-3FC54B1A15F8}"/>
+    <hyperlink ref="C56" r:id="rId15" xr:uid="{1A254817-AA29-4349-9F3D-1F08E4B7BC6D}"/>
+    <hyperlink ref="C63" r:id="rId16" location="{Reactor_type}Reactor" xr:uid="{0AB9E7B4-D674-2E47-9B72-341D1022B491}"/>
+    <hyperlink ref="C57" r:id="rId17" location="{Reaction_medium}Medium" xr:uid="{9FFFB41F-40DA-E844-8105-33FA71783875}"/>
+    <hyperlink ref="C58" r:id="rId18" location="{Operation_mode}Mode" xr:uid="{E49C1ABB-2410-D945-BAD5-E813751ECA22}"/>
+    <hyperlink ref="C70" r:id="rId19" location="{Light_source}LightSource" xr:uid="{5D5BAA03-A593-D246-AA1D-DD5A58EEB0FF}"/>
+    <hyperlink ref="C71" r:id="rId20" location="{Lamp}Lamp" xr:uid="{B474DE65-6CF2-6449-8CB9-C1A8F1227029}"/>
+    <hyperlink ref="C72" r:id="rId21" location="{Wavelength_nm}WL" xr:uid="{CDAAFAD0-E55A-C64F-A0E5-874107AAA07C}"/>
+    <hyperlink ref="C73" r:id="rId22" xr:uid="{D635B011-750E-414E-91E7-5327241CF37A}"/>
+    <hyperlink ref="C74:C75" r:id="rId23" display="http://w3id.org/solar/i/IlluminatedArea/{ID}" xr:uid="{4DFEDC35-DAA6-804C-B0F6-2CAF9BC91727}"/>
+    <hyperlink ref="C74" r:id="rId24" xr:uid="{1D48B95E-8BAD-E044-A7A5-74EFE823C221}"/>
+    <hyperlink ref="C75" r:id="rId25" xr:uid="{6118BC49-CEA9-7C4E-ABE8-63EA5ED604C9}"/>
+    <hyperlink ref="C49" r:id="rId26" xr:uid="{BD436ABE-9765-184F-AB49-2AAD056EA2AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId19"/>
+  <legacyDrawing r:id="rId27"/>
 </worksheet>
 </file>
 

</xml_diff>